<commit_message>
mobile responsive bug fixed
</commit_message>
<xml_diff>
--- a/HHM-Support.xlsx
+++ b/HHM-Support.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\git\hhm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE81910-6A56-4622-B076-2FCA7B9DE7C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A509E52-0EA5-4136-B5A5-0BBFCF1B911B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{1E86B32A-A4E6-46A4-A9E6-3A88B75D608F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
   <si>
     <t>HHM PURE SUPPORT HOURS</t>
   </si>
@@ -178,7 +178,13 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -188,12 +194,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -518,7 +518,7 @@
   <dimension ref="F3:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,44 +527,44 @@
   </cols>
   <sheetData>
     <row r="3" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
     </row>
     <row r="4" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
     </row>
     <row r="5" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
     </row>
     <row r="7" spans="6:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18" t="s">
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="18"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="6:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F8" s="4"/>
@@ -575,24 +575,24 @@
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="6:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="11" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F11" s="2">
         <v>6</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
       <c r="J11" s="7">
         <v>0.125</v>
       </c>
@@ -604,11 +604,11 @@
       <c r="F12" s="3">
         <v>7</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
       <c r="J12" s="7">
         <v>0.125</v>
       </c>
@@ -620,11 +620,11 @@
       <c r="F13">
         <v>9</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
       <c r="J13" s="7">
         <v>6.25E-2</v>
       </c>
@@ -636,11 +636,11 @@
       <c r="F14">
         <v>10</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
       <c r="J14" s="7">
         <v>0.16666666666666666</v>
       </c>
@@ -652,11 +652,11 @@
       <c r="F15">
         <v>11</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
       <c r="J15" s="7">
         <v>0.16666666666666666</v>
       </c>
@@ -668,11 +668,11 @@
       <c r="F16">
         <v>12</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
       <c r="J16" s="7">
         <v>0.16666666666666666</v>
       </c>
@@ -684,11 +684,11 @@
       <c r="F17">
         <v>13</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
       <c r="J17" s="7">
         <v>6.25E-2</v>
       </c>
@@ -700,11 +700,11 @@
       <c r="F18">
         <v>15</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
       <c r="J18" s="7">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -716,11 +716,11 @@
       <c r="F19">
         <v>16</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
       <c r="J19" s="7">
         <v>0.10416666666666667</v>
       </c>
@@ -732,11 +732,11 @@
       <c r="F20">
         <v>19</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
       <c r="J20" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -748,11 +748,11 @@
       <c r="F21">
         <v>20</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
       <c r="J21" s="7">
         <v>0.10416666666666667</v>
       </c>
@@ -764,11 +764,11 @@
       <c r="F22">
         <v>21</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
       <c r="J22" s="7">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -780,11 +780,11 @@
       <c r="F23">
         <v>25</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
       <c r="J23" s="7">
         <v>8.3333333333333301E-2</v>
       </c>
@@ -796,11 +796,11 @@
       <c r="F24">
         <v>26</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
       <c r="J24" s="7">
         <v>0.20833333333333334</v>
       </c>
@@ -812,11 +812,11 @@
       <c r="F25">
         <v>27</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
       <c r="J25" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -828,11 +828,11 @@
       <c r="F26">
         <v>29</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
       <c r="J26" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -844,11 +844,11 @@
       <c r="F27">
         <v>30</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
       <c r="J27" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -865,11 +865,11 @@
     </row>
     <row r="29" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F29" s="6"/>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
       <c r="J29" s="8">
         <f>SUM(J11:J27)</f>
         <v>1.7291666666666663</v>
@@ -895,14 +895,14 @@
       <c r="K31" s="11"/>
     </row>
     <row r="32" spans="6:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F32" s="19" t="s">
+      <c r="F32" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
     </row>
     <row r="33" spans="6:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F33" s="10"/>
@@ -916,11 +916,11 @@
       <c r="F34">
         <v>2</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
       <c r="J34" s="7">
         <v>0.25</v>
       </c>
@@ -932,11 +932,11 @@
       <c r="F35">
         <v>3</v>
       </c>
-      <c r="G35" s="15" t="s">
+      <c r="G35" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
       <c r="J35" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -944,38 +944,39 @@
         <v>6</v>
       </c>
     </row>
+    <row r="36" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="38" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F38" s="6"/>
-      <c r="G38" s="20" t="s">
+      <c r="G38" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
       <c r="J38" s="8">
         <f>SUM(J34:J37)</f>
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="K38" s="6" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+  <mergeCells count="27">
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="F3:K5"/>
     <mergeCell ref="G7:I7"/>
@@ -987,6 +988,22 @@
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="F9:K9"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G36:I36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>